<commit_message>
suppression durée traitement 8d6f0c39f0988860ec16f4ac7fe387dbf9240836
</commit_message>
<xml_diff>
--- a/nr-add-poso-logical-model/ig/StructureDefinition-fr-posologie.xlsx
+++ b/nr-add-poso-logical-model/ig/StructureDefinition-fr-posologie.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="165">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-18T15:58:54+00:00</t>
+    <t>2025-07-21T07:18:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -503,28 +503,10 @@
     <t>Date précise du moment de prise</t>
   </si>
   <si>
-    <t>fr-posologie.dureeTraitement</t>
-  </si>
-  <si>
-    <t>Durée du traitement - la durée du traitement peut être indiquée en complément ou à la place des dates de début et de fin de traitement</t>
-  </si>
-  <si>
-    <t>fr-posologie.dureeTraitement.valeur</t>
-  </si>
-  <si>
-    <t>Valeur de la durée de traitement</t>
-  </si>
-  <si>
-    <t>fr-posologie.dureeTraitement.unite</t>
-  </si>
-  <si>
-    <t>Unité de la durée de traitement</t>
-  </si>
-  <si>
     <t>fr-posologie.momentDePrise</t>
   </si>
   <si>
-    <t>moment de la prise au cours de la journée (ex : 30 minutes avant le repas)</t>
+    <t>Définition du moment de prise au cours de la journée (ex : 30 minutes avant le repas)</t>
   </si>
   <si>
     <t>fr-posologie.momentDePrise.code</t>
@@ -845,7 +827,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ42"/>
+  <dimension ref="A1:AJ39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -4417,7 +4399,7 @@
         <v>72</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>19</v>
@@ -4492,7 +4474,7 @@
         <v>72</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>19</v>
@@ -4517,7 +4499,7 @@
         <v>72</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>19</v>
@@ -4592,7 +4574,7 @@
         <v>72</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>19</v>
@@ -4629,7 +4611,7 @@
         <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="L38" t="s" s="2">
         <v>161</v>
@@ -4729,13 +4711,13 @@
         <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -4798,306 +4780,6 @@
         <v>19</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="H40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q40" s="2"/>
-      <c r="R40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="H41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="2"/>
-      <c r="R41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="G42" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q42" s="2"/>
-      <c r="R42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add increment & improve text ab19e80cfcb967e46d742a9c57df62a6c5a22404
</commit_message>
<xml_diff>
--- a/nr-add-poso-logical-model/ig/StructureDefinition-fr-posologie.xlsx
+++ b/nr-add-poso-logical-model/ig/StructureDefinition-fr-posologie.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-21T07:18:37+00:00</t>
+    <t>2025-07-21T07:29:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -274,7 +274,7 @@
 QuantityRange</t>
   </si>
   <si>
-    <t>Durée pendant laquel une dose définie est administére  (pendant 1 heure, entre 5 et 10 minutes)</t>
+    <t>Durée pendant laquelle une dose définie est administrée  (pendant 1 heure, entre 5 et 10 minutes)</t>
   </si>
   <si>
     <t>fr-posologie.sequence</t>
@@ -284,7 +284,7 @@
 </t>
   </si>
   <si>
-    <t>Numéro de séquence. La séquence s+1 commence à la fin de la séquence s. En cas de séquences ayant le même numéro, celles-ci se déroulent simultanément.</t>
+    <t>Numéro de séquence permettant d'indiquer l'ordre des posologies dans le cas où il y a plusieurs posologies. La séquence s+1 commence à la fin de la séquence s. En cas de séquences ayant le même numéro, celles-ci se déroulent simultanément.</t>
   </si>
   <si>
     <t>fr-posologie.evenementFinSequence</t>
@@ -432,7 +432,7 @@
     <t>fr-posologie.dureeAdministration</t>
   </si>
   <si>
-    <t>Rythme d'administration</t>
+    <t>Durée ou rythme d'administration - indique le temps d'administration (ex - perfusion pendant 10 minutes)</t>
   </si>
   <si>
     <t>fr-posologie.dureeAdministration.duree</t>
@@ -480,7 +480,7 @@
 </t>
   </si>
   <si>
-    <t>Durée du traitement</t>
+    <t>Durée du traitement (ex : pendant 5 jours)</t>
   </si>
   <si>
     <t>fr-posologie.dateRange</t>

</xml_diff>